<commit_message>
created new sheet and added data on it
</commit_message>
<xml_diff>
--- a/SabeloCalc.xlsx
+++ b/SabeloCalc.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Trainee Roster" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -19,16 +20,195 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <si>
+    <t xml:space="preserve">Trainee ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Msizi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gumede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msizi@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zanele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zikode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zikode@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gregory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Govender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">govender@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mpume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mpungose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpungose@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sbonelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zondo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zondo@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sobahle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sobahle@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qiniso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pungwayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qiniso@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xolani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dlamini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xolani@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lindelani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hlongwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lindelani@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khuselo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joli@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0732341243</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -44,6 +224,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,8 +282,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -218,7 +432,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -232,4 +446,331 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.74"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>38855</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="true">DATEDIF(F2, TODAY(), "Y")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>36665</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="true">DATEDIF(F3, TODAY(), "Y")</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>39222</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="true">DATEDIF(F4, TODAY(), "Y")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>35206</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="true">DATEDIF(F5, TODAY(), "Y")</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>32650</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="true">DATEDIF(F6, TODAY(), "Y")</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>33016</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="true">DATEDIF(F7, TODAY(), "Y")</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>37035</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="true">DATEDIF(F8, TODAY(), "Y")</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>37401</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="true">DATEDIF(F9, TODAY(), "Y")</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>36672</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="true">DATEDIF(F10, TODAY(), "Y")</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>37768</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <f aca="true">DATEDIF(F11, TODAY(), "Y")</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="msizi@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="zikode@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="govender@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId4" display="mpungose@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId5" display="zondo@gmail.com"/>
+    <hyperlink ref="D7" r:id="rId6" display="sobahle@gmail.com"/>
+    <hyperlink ref="D8" r:id="rId7" display="qiniso@gmail.com"/>
+    <hyperlink ref="D9" r:id="rId8" display="xolani@gmail.com"/>
+    <hyperlink ref="D10" r:id="rId9" display="lindelani@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>